<commit_message>
Recursive sorting by name and qty completed
</commit_message>
<xml_diff>
--- a/inventory_original.xlsx
+++ b/inventory_original.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t>Product Type</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Large</t>
+  </si>
+  <si>
+    <t>Machine</t>
   </si>
 </sst>
 </file>
@@ -557,11 +560,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
+      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,7 +578,7 @@
     <col min="9" max="10" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,8 +618,11 @@
       <c r="M1" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -647,8 +653,11 @@
       <c r="K2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -679,8 +688,11 @@
       <c r="K3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -711,8 +723,11 @@
       <c r="K4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -743,8 +758,11 @@
       <c r="K5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -775,8 +793,11 @@
       <c r="K6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -807,8 +828,11 @@
       <c r="K7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -839,8 +863,11 @@
       <c r="K8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -871,8 +898,11 @@
       <c r="K9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -906,8 +936,11 @@
       <c r="K10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -941,8 +974,11 @@
       <c r="K11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -976,8 +1012,11 @@
       <c r="K12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1011,8 +1050,11 @@
       <c r="K13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1046,8 +1088,11 @@
       <c r="K14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1084,8 +1129,11 @@
       <c r="M15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1122,8 +1170,11 @@
       <c r="M16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1159,6 +1210,9 @@
       </c>
       <c r="M17" t="b">
         <v>0</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>